<commit_message>
predict round of last 16
</commit_message>
<xml_diff>
--- a/data/input/matches.xlsx
+++ b/data/input/matches.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="34">
   <si>
     <t xml:space="preserve">Stage</t>
   </si>
@@ -230,8 +230,8 @@
   </sheetPr>
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E45" activeCellId="0" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -872,40 +872,88 @@
       <c r="A38" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="B38" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="B39" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="B40" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="B41" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="B42" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="B43" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="B44" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>30</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>